<commit_message>
:memo: modified md file
</commit_message>
<xml_diff>
--- a/WBS.xlsx
+++ b/WBS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Document\project\01_GitHub\06_Plz_Take_care_of_My_Refrigerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8AA336-E2DF-478C-902C-F9BA1D17D2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A11C401-9FBA-45EA-B334-229265B5D900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{958269B8-2A52-4794-8B3D-464A21221AA4}"/>
+    <workbookView xWindow="51560" yWindow="0" windowWidth="15730" windowHeight="20970" xr2:uid="{958269B8-2A52-4794-8B3D-464A21221AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
@@ -1156,6 +1156,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1198,9 +1201,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1219,28 +1219,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1560,11 +1560,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADACCCB8-0ADB-4200-A097-9BD4AB4DC274}">
   <dimension ref="B2:O51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:O2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -1583,62 +1583,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.6">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="47" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="49"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.6">
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="49" t="s">
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="49" t="s">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="52"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="53"/>
     </row>
     <row r="5" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B5" s="18" t="s">
@@ -1685,10 +1685,10 @@
       </c>
     </row>
     <row r="6" spans="2:15" ht="17.25" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="4" t="s">
         <v>46</v>
       </c>
@@ -1707,10 +1707,10 @@
       <c r="O6" s="7"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.6">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="40"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="4" t="s">
         <v>42</v>
       </c>
@@ -1729,10 +1729,10 @@
       <c r="O7" s="7"/>
     </row>
     <row r="8" spans="2:15" ht="33.75" x14ac:dyDescent="0.6">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="17" t="s">
         <v>106</v>
       </c>
@@ -1757,10 +1757,10 @@
       <c r="O8" s="7"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.6">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="40"/>
+      <c r="C9" s="41"/>
       <c r="D9" s="4"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
@@ -2019,10 +2019,10 @@
       <c r="O21" s="8"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.6">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="1" t="s">
         <v>45</v>
       </c>
@@ -2081,10 +2081,10 @@
       <c r="O24" s="8"/>
     </row>
     <row r="25" spans="2:15" ht="33.75" x14ac:dyDescent="0.6">
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="40"/>
+      <c r="C25" s="41"/>
       <c r="D25" s="20" t="s">
         <v>47</v>
       </c>
@@ -2163,10 +2163,10 @@
       <c r="O28" s="8"/>
     </row>
     <row r="29" spans="2:15" ht="33.75" x14ac:dyDescent="0.6">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="40"/>
+      <c r="C29" s="41"/>
       <c r="D29" s="20" t="s">
         <v>48</v>
       </c>
@@ -2425,10 +2425,10 @@
       <c r="O38" s="8"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.6">
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="40"/>
+      <c r="C39" s="41"/>
       <c r="D39" s="1" t="s">
         <v>49</v>
       </c>
@@ -2631,10 +2631,10 @@
       <c r="O46" s="8"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.6">
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="40"/>
+      <c r="C47" s="41"/>
       <c r="D47" s="1" t="s">
         <v>50</v>
       </c>
@@ -2718,7 +2718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A39BF2A-795A-45A8-8F54-B37C3C9698E8}">
   <dimension ref="B2:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
@@ -2736,68 +2736,68 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.6">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="47" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="49"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.6">
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="49" t="s">
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="50"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="49" t="s">
+      <c r="L4" s="51"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="52"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="53"/>
     </row>
     <row r="5" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B5" s="18" t="s">
@@ -2850,10 +2850,10 @@
       </c>
     </row>
     <row r="6" spans="2:17" ht="17.25" thickTop="1" x14ac:dyDescent="0.6">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -2872,7 +2872,7 @@
       <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.6">
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="62" t="s">
         <v>103</v>
       </c>
       <c r="C7" s="56" t="s">
@@ -3503,8 +3503,8 @@
     </row>
     <row r="27" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B27" s="64"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="60"/>
       <c r="E27" s="9" t="s">
         <v>99</v>
       </c>
@@ -3532,13 +3532,13 @@
       <c r="Q27" s="10"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.6">
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="65" t="s">
+      <c r="C28" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="67" t="s">
         <v>31</v>
       </c>
       <c r="E28" s="33" t="s">
@@ -4163,8 +4163,8 @@
     </row>
     <row r="48" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B48" s="64"/>
-      <c r="C48" s="60"/>
-      <c r="D48" s="61"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="60"/>
       <c r="E48" s="9" t="s">
         <v>99</v>
       </c>
@@ -4192,13 +4192,13 @@
       <c r="Q48" s="10"/>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.6">
-      <c r="B49" s="62" t="s">
+      <c r="B49" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="65" t="s">
+      <c r="C49" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="66" t="s">
+      <c r="D49" s="67" t="s">
         <v>31</v>
       </c>
       <c r="E49" s="33" t="s">
@@ -4823,8 +4823,8 @@
     </row>
     <row r="69" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B69" s="64"/>
-      <c r="C69" s="60"/>
-      <c r="D69" s="61"/>
+      <c r="C69" s="61"/>
+      <c r="D69" s="60"/>
       <c r="E69" s="9" t="s">
         <v>99</v>
       </c>
@@ -4853,37 +4853,10 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:J4"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="B7:B27"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="C9:C18"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C40:C45"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="C30:C39"/>
-    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C61:C66"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D65:D66"/>
     <mergeCell ref="C67:C69"/>
     <mergeCell ref="D67:D69"/>
     <mergeCell ref="C46:C48"/>
@@ -4900,10 +4873,37 @@
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="D59:D60"/>
-    <mergeCell ref="C61:C66"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="C40:C45"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="C30:C39"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="B7:B27"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C9:C18"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:J4"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:Q4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>